<commit_message>
update excel and csv
</commit_message>
<xml_diff>
--- a/templates/csv/list_remain.xlsx
+++ b/templates/csv/list_remain.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="681">
   <si>
     <t>000032</t>
   </si>
@@ -2067,9 +2067,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>q</t>
   </si>
 </sst>
 </file>
@@ -2424,7 +2421,7 @@
   <dimension ref="A1:P673"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,9 +2562,6 @@
         <f t="shared" si="0"/>
         <v>3056808</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>681</v>
-      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">

</xml_diff>